<commit_message>
Modified to load csgo data from steamdb repo
</commit_message>
<xml_diff>
--- a/SteamInventoryManager.Console/reports/StorageUnitTemplate.xlsx
+++ b/SteamInventoryManager.Console/reports/StorageUnitTemplate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\shazan\SteamInventoryManager\SteamInventoryManager.Console\reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{980B1E7B-82B5-48C7-A552-B1BB9D3B0371}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA8671AA-5E85-4CF2-AA8A-1987A63AC4A5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{46EBE0E3-8D9C-4F2D-83A6-199D6AFB2824}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="CSGOitems">Sheet1!$B$10:$Q$11</definedName>
+    <definedName name="CSGOitems">Sheet1!$B$10:$N$11</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
   <si>
     <t>Storage Unit Name :</t>
   </si>
@@ -65,9 +65,6 @@
     <t>&lt;&lt;sum&gt;&gt;</t>
   </si>
   <si>
-    <t>Value</t>
-  </si>
-  <si>
     <t>{{name}}</t>
   </si>
   <si>
@@ -83,9 +80,6 @@
     <t>{{item.IsSpray}}</t>
   </si>
   <si>
-    <t>{{item.Value}}</t>
-  </si>
-  <si>
     <t>{{item.MarketName}}</t>
   </si>
   <si>
@@ -95,9 +89,6 @@
     <t>{{item.Quantity}}</t>
   </si>
   <si>
-    <t>Username:</t>
-  </si>
-  <si>
     <t>{{username}}</t>
   </si>
   <si>
@@ -105,6 +96,27 @@
   </si>
   <si>
     <t>{{item.Float}}</t>
+  </si>
+  <si>
+    <t>Tradeable</t>
+  </si>
+  <si>
+    <t>{{item.IsTradeable}}</t>
+  </si>
+  <si>
+    <t>Steam Value</t>
+  </si>
+  <si>
+    <t>Buff163 Value</t>
+  </si>
+  <si>
+    <t>{{item.Buff163Value}}</t>
+  </si>
+  <si>
+    <t>{{item.SteamValue}}</t>
+  </si>
+  <si>
+    <t>Steam ID:</t>
   </si>
 </sst>
 </file>
@@ -187,7 +199,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -225,19 +237,6 @@
     </border>
     <border>
       <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right/>
       <top style="thin">
         <color indexed="64"/>
@@ -249,7 +248,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -264,19 +263,25 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -285,7 +290,7 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -294,16 +299,16 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -620,171 +625,152 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6D3290C-18F6-4177-877A-265A510F08E2}">
-  <dimension ref="B3:Q12"/>
+  <dimension ref="B3:N12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4" customWidth="1"/>
-    <col min="5" max="5" width="33.5703125" customWidth="1"/>
-    <col min="6" max="6" width="22.28515625" customWidth="1"/>
-    <col min="8" max="8" width="16" customWidth="1"/>
+    <col min="5" max="5" width="19.7109375" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" customWidth="1"/>
+    <col min="7" max="7" width="16.28515625" customWidth="1"/>
+    <col min="8" max="8" width="21.5703125" customWidth="1"/>
     <col min="9" max="9" width="18.85546875" customWidth="1"/>
-    <col min="10" max="10" width="9.85546875" customWidth="1"/>
-    <col min="11" max="11" width="11.85546875" customWidth="1"/>
-    <col min="13" max="13" width="12.42578125" customWidth="1"/>
-    <col min="15" max="15" width="22.28515625" customWidth="1"/>
+    <col min="10" max="10" width="21" customWidth="1"/>
+    <col min="11" max="11" width="16.140625" customWidth="1"/>
+    <col min="12" max="12" width="21.42578125" customWidth="1"/>
+    <col min="13" max="13" width="24.28515625" customWidth="1"/>
+    <col min="14" max="14" width="24.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:17" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="I3" s="8" t="s">
+    <row r="3" spans="2:14" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="I3" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="8"/>
-      <c r="M3" s="8"/>
-      <c r="N3" s="8"/>
+      <c r="J3" s="21"/>
+      <c r="K3" s="21"/>
+      <c r="L3" s="21"/>
     </row>
-    <row r="6" spans="2:17" ht="21" x14ac:dyDescent="0.35">
-      <c r="B6" s="7" t="s">
+    <row r="6" spans="2:14" ht="21" x14ac:dyDescent="0.35">
+      <c r="B6" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" s="19"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
-      <c r="K6" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="L6" s="11"/>
-      <c r="M6" s="11"/>
-      <c r="N6" s="12" t="s">
+      <c r="K6" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="L6" s="14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="2:14" ht="21" x14ac:dyDescent="0.35">
+      <c r="B9" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="19"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="G9" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="H9" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="O6" s="12"/>
-    </row>
-    <row r="9" spans="2:17" ht="21" x14ac:dyDescent="0.35">
-      <c r="B9" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="C9" s="15"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="G9" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="H9" s="15"/>
       <c r="I9" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="J9" s="9" t="s">
+      <c r="J9" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="K9" s="10"/>
-      <c r="L9" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="M9" s="10"/>
-      <c r="N9" s="9" t="s">
+      <c r="K9" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="L9" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="O9" s="10"/>
-      <c r="P9" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="Q9" s="10"/>
+      <c r="M9" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="N9" s="8" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="10" spans="2:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B10" s="14" t="s">
+    <row r="10" spans="2:14" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B10" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G10" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="J10" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="K10" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="G10" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="H10" s="14"/>
-      <c r="I10" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="J10" s="16" t="s">
+      <c r="L10" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="K10" s="17"/>
-      <c r="L10" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="M10" s="17"/>
-      <c r="N10" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="O10" s="17"/>
-      <c r="P10" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q10" s="17"/>
+      <c r="M10" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="N10" s="9" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="11" spans="2:17" ht="21" x14ac:dyDescent="0.35">
-      <c r="J11" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="K11" s="6"/>
-      <c r="L11" s="13" t="s">
+    <row r="11" spans="2:14" ht="21" x14ac:dyDescent="0.35">
+      <c r="J11" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="K11" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="M11" s="13"/>
-      <c r="N11" s="6" t="s">
+      <c r="L11" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="O11" s="6"/>
-      <c r="P11" s="18" t="s">
+      <c r="M11" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="Q11" s="18"/>
+      <c r="N11" s="10" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="12" spans="2:17" ht="21" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:14" ht="21" x14ac:dyDescent="0.35">
       <c r="I12" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="21">
-    <mergeCell ref="P9:Q9"/>
-    <mergeCell ref="P10:Q10"/>
-    <mergeCell ref="P11:Q11"/>
-    <mergeCell ref="L9:M9"/>
-    <mergeCell ref="L10:M10"/>
-    <mergeCell ref="N10:O10"/>
-    <mergeCell ref="N11:O11"/>
+  <mergeCells count="4">
     <mergeCell ref="B6:D6"/>
-    <mergeCell ref="I3:N3"/>
-    <mergeCell ref="N9:O9"/>
-    <mergeCell ref="K6:M6"/>
-    <mergeCell ref="N6:O6"/>
-    <mergeCell ref="L11:M11"/>
-    <mergeCell ref="J11:K11"/>
+    <mergeCell ref="I3:L3"/>
     <mergeCell ref="B10:E10"/>
     <mergeCell ref="B9:E9"/>
-    <mergeCell ref="J9:K9"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="E6:F6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated new changes and fixes
</commit_message>
<xml_diff>
--- a/SteamInventoryManager.Console/reports/StorageUnitTemplate.xlsx
+++ b/SteamInventoryManager.Console/reports/StorageUnitTemplate.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\shazan\SteamInventoryManager\SteamInventoryManager.Console\reports\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\shazan\SteamInventoryManager\SteamInventoryManager.Console\bin\Debug\net5.0\reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA8671AA-5E85-4CF2-AA8A-1987A63AC4A5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22B5134D-696D-4D6F-95CB-76228F341421}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{46EBE0E3-8D9C-4F2D-83A6-199D6AFB2824}"/>
   </bookViews>
@@ -123,6 +123,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+  </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -248,7 +251,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -275,9 +278,6 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -299,16 +299,22 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -627,8 +633,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6D3290C-18F6-4177-877A-265A510F08E2}">
   <dimension ref="B3:N12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -647,20 +653,20 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:14" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="I3" s="21" t="s">
+      <c r="I3" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="J3" s="21"/>
-      <c r="K3" s="21"/>
-      <c r="L3" s="21"/>
+      <c r="J3" s="18"/>
+      <c r="K3" s="18"/>
+      <c r="L3" s="18"/>
     </row>
     <row r="6" spans="2:14" ht="21" x14ac:dyDescent="0.35">
-      <c r="B6" s="20" t="s">
+      <c r="B6" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="20"/>
-      <c r="D6" s="20"/>
-      <c r="E6" s="15" t="s">
+      <c r="C6" s="17"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="14" t="s">
         <v>10</v>
       </c>
       <c r="F6" s="1"/>
@@ -668,24 +674,24 @@
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
-      <c r="K6" s="13" t="s">
+      <c r="K6" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="L6" s="14" t="s">
+      <c r="L6" s="13" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="9" spans="2:14" ht="21" x14ac:dyDescent="0.35">
-      <c r="B9" s="19" t="s">
+      <c r="B9" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="19"/>
-      <c r="D9" s="19"/>
-      <c r="E9" s="19"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
       <c r="F9" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="G9" s="17" t="s">
+      <c r="G9" s="16" t="s">
         <v>5</v>
       </c>
       <c r="H9" s="7" t="s">
@@ -711,16 +717,16 @@
       </c>
     </row>
     <row r="10" spans="2:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B10" s="18" t="s">
+      <c r="B10" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="18"/>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="19"/>
       <c r="F10" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="G10" s="16" t="s">
+      <c r="G10" s="15" t="s">
         <v>7</v>
       </c>
       <c r="H10" s="6" t="s">
@@ -738,27 +744,27 @@
       <c r="L10" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="M10" s="9" t="s">
+      <c r="M10" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="N10" s="9" t="s">
+      <c r="N10" s="21" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="11" spans="2:14" ht="21" x14ac:dyDescent="0.35">
-      <c r="J11" s="11" t="s">
+      <c r="J11" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="K11" s="12" t="s">
+      <c r="K11" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="L11" s="11" t="s">
+      <c r="L11" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="M11" s="10" t="s">
+      <c r="M11" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="N11" s="10" t="s">
+      <c r="N11" s="22" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>